<commit_message>
did more practices and added questions
</commit_message>
<xml_diff>
--- a/src/com/practice/interview/InterviewQuestions (DSAndAlgos).xlsx
+++ b/src/com/practice/interview/InterviewQuestions (DSAndAlgos).xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
   <si>
     <t>Topic</t>
   </si>
@@ -69,13 +69,61 @@
     <t>What is balanced binary tree?</t>
   </si>
   <si>
-    <t>https://www.interviewcake.com/concept/java/bfs</t>
-  </si>
-  <si>
-    <t>https://www.interviewcake.com/concept/java/dfs</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=LU4fGD-fgJQ</t>
+  </si>
+  <si>
+    <t>What DS is used for BFS?</t>
+  </si>
+  <si>
+    <t>Queue</t>
+  </si>
+  <si>
+    <t>What DS is used for DFS?</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>Graph</t>
+  </si>
+  <si>
+    <t>What is BFS and DFS spanning tree?</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=pcKY4hjDrxk</t>
+  </si>
+  <si>
+    <t>Algorithms</t>
+  </si>
+  <si>
+    <t>What is algorithm?</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=0IAPZzGSbME&amp;list=PLDN4rrl48XKpZkf03iYFl-O29szjTrs_O&amp;index=1</t>
+  </si>
+  <si>
+    <t>Difference between algorithm and program?</t>
+  </si>
+  <si>
+    <t>What is priori analysis?</t>
+  </si>
+  <si>
+    <t>What is asymptotic notation?</t>
+  </si>
+  <si>
+    <t>How many asymptotic notations do we have?</t>
+  </si>
+  <si>
+    <t>What are the properties of asymptotic notation?</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=NI4OKSvGAgM&amp;list=PLDN4rrl48XKpZkf03iYFl-O29szjTrs_O&amp;index=13</t>
+  </si>
+  <si>
+    <t>How many ways we can search elements in an array?</t>
+  </si>
+  <si>
+    <t>What is disjoint set?</t>
   </si>
 </sst>
 </file>
@@ -442,18 +490,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="90.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -475,13 +523,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -489,13 +537,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -592,19 +640,132 @@
         <v>16</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="C22" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D9" r:id="rId1"/>
     <hyperlink ref="D8" r:id="rId2"/>
-    <hyperlink ref="D2" r:id="rId3"/>
-    <hyperlink ref="D3" r:id="rId4"/>
-    <hyperlink ref="D11" r:id="rId5"/>
+    <hyperlink ref="D11" r:id="rId3"/>
+    <hyperlink ref="D14" r:id="rId4"/>
+    <hyperlink ref="D2" r:id="rId5"/>
+    <hyperlink ref="D3" r:id="rId6"/>
+    <hyperlink ref="D15" r:id="rId7"/>
+    <hyperlink ref="D16" r:id="rId8"/>
+    <hyperlink ref="D20" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added more questions and TODO task
</commit_message>
<xml_diff>
--- a/src/com/practice/interview/InterviewQuestions (DSAndAlgos).xlsx
+++ b/src/com/practice/interview/InterviewQuestions (DSAndAlgos).xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="39">
   <si>
     <t>Topic</t>
   </si>
@@ -124,6 +124,18 @@
   </si>
   <si>
     <t>What is disjoint set?</t>
+  </si>
+  <si>
+    <t>What is general form of recurrance solution?</t>
+  </si>
+  <si>
+    <t>aT(n-b)+f(n) when a &gt; 0, b &gt; 0 and f(n) = O(n^k) where k &gt;= 0
+if a=1 then  O(n^(k+1)) or O(n*f(n))
+if a &gt; 1 then O(n^K * a^(n/b)) or O(f(n) * a^(n/b))
+if a &lt; 1 then O(n^k) or O(f(n))</t>
+  </si>
+  <si>
+    <t>What is masters theorem for decreasing functions?</t>
   </si>
 </sst>
 </file>
@@ -191,10 +203,13 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -490,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -743,13 +758,38 @@
       </c>
     </row>
     <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
       <c r="C21" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
       <c r="C22" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="60">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some interview questions
</commit_message>
<xml_diff>
--- a/src/com/practice/interview/InterviewQuestions (DSAndAlgos).xlsx
+++ b/src/com/practice/interview/InterviewQuestions (DSAndAlgos).xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="41">
   <si>
     <t>Topic</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>What is masters theorem for decreasing functions?</t>
+  </si>
+  <si>
+    <t>What is general form of recurrance solution for dividing functions?</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=OynWkEj0S-s&amp;list=PLDN4rrl48XKpZkf03iYFl-O29szjTrs_O&amp;index=27</t>
   </si>
 </sst>
 </file>
@@ -203,11 +209,14 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -505,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -792,6 +801,17 @@
         <v>38</v>
       </c>
     </row>
+    <row r="25" spans="1:4" ht="30">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D9" r:id="rId1"/>
@@ -803,9 +823,10 @@
     <hyperlink ref="D15" r:id="rId7"/>
     <hyperlink ref="D16" r:id="rId8"/>
     <hyperlink ref="D20" r:id="rId9"/>
+    <hyperlink ref="D25" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added different sorting techniques
</commit_message>
<xml_diff>
--- a/src/com/practice/interview/InterviewQuestions (DSAndAlgos).xlsx
+++ b/src/com/practice/interview/InterviewQuestions (DSAndAlgos).xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="43">
   <si>
     <t>Topic</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=OynWkEj0S-s&amp;list=PLDN4rrl48XKpZkf03iYFl-O29szjTrs_O&amp;index=27</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=HqPJF2L5h9U&amp;t=4s</t>
+  </si>
+  <si>
+    <t>What is max and min heap?</t>
   </si>
 </sst>
 </file>
@@ -514,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -652,6 +658,9 @@
       <c r="C10" t="s">
         <v>15</v>
       </c>
+      <c r="D10" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
@@ -810,6 +819,14 @@
       </c>
       <c r="D25" s="4" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="C26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -824,9 +841,11 @@
     <hyperlink ref="D16" r:id="rId8"/>
     <hyperlink ref="D20" r:id="rId9"/>
     <hyperlink ref="D25" r:id="rId10"/>
+    <hyperlink ref="D10" r:id="rId11"/>
+    <hyperlink ref="D26" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 

</xml_diff>